<commit_message>
pm_pcsgen: Fix the description of 'symmetrical' in pm_pcsgen_sample.xlsx
</commit_message>
<xml_diff>
--- a/pm_pcsgen/pm_pcsgen_sample.xlsx
+++ b/pm_pcsgen/pm_pcsgen_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ka_inoue\Desktop\telwork\UPD\4660\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ka_inoue\Desktop\telwork\UPD\4802_4786\4786\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2122,25 +2122,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>起動と逆順に停止</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(y/n)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>#</t>
     </r>
     <r>
@@ -2597,6 +2578,26 @@
       </rPr>
       <t>の実行順序</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>起動と逆順に停止</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(true/false)</t>
+    </r>
+    <phoneticPr fontId="7"/>
   </si>
 </sst>
 </file>
@@ -11689,7 +11690,7 @@
       </c>
       <c r="L223" s="128"/>
       <c r="M223" s="49" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="N223" s="66" t="s">
         <v>201</v>
@@ -11763,7 +11764,7 @@
     </row>
     <row r="228" spans="1:14" ht="14.45" customHeight="1">
       <c r="A228" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
@@ -11823,7 +11824,7 @@
       </c>
       <c r="B231" s="26"/>
       <c r="C231" s="121" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D231" s="121"/>
       <c r="E231" s="121"/>
@@ -11960,7 +11961,7 @@
       </c>
       <c r="B238" s="26"/>
       <c r="C238" s="114" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D238" s="114"/>
       <c r="E238" s="114"/>
@@ -12097,7 +12098,7 @@
       </c>
       <c r="B245" s="26"/>
       <c r="C245" s="114" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D245" s="114"/>
       <c r="E245" s="114"/>
@@ -12225,7 +12226,7 @@
     </row>
     <row r="252" spans="1:14" ht="14.45" customHeight="1">
       <c r="A252" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
@@ -12283,7 +12284,7 @@
       </c>
       <c r="B255" s="2"/>
       <c r="C255" s="100" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D255" s="100"/>
       <c r="E255" s="100"/>
@@ -12364,7 +12365,7 @@
         <v>5</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
@@ -12384,7 +12385,7 @@
         <v>5</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
@@ -13914,7 +13915,7 @@
       <c r="J39" s="124"/>
       <c r="K39" s="124"/>
       <c r="L39" s="208" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M39" s="208"/>
       <c r="N39" s="208"/>
@@ -14324,7 +14325,7 @@
     </row>
     <row r="61" spans="1:14" ht="14.45" customHeight="1">
       <c r="A61" s="84" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -18679,7 +18680,7 @@
       </c>
       <c r="L259" s="128"/>
       <c r="M259" s="49" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="N259" s="66" t="s">
         <v>201</v>
@@ -18775,7 +18776,7 @@
     </row>
     <row r="264" spans="1:14" ht="14.45" customHeight="1">
       <c r="A264" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
@@ -18835,7 +18836,7 @@
       </c>
       <c r="B267" s="26"/>
       <c r="C267" s="121" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D267" s="121"/>
       <c r="E267" s="121"/>
@@ -18972,7 +18973,7 @@
       </c>
       <c r="B274" s="26"/>
       <c r="C274" s="114" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D274" s="114"/>
       <c r="E274" s="114"/>
@@ -19109,7 +19110,7 @@
       </c>
       <c r="B281" s="26"/>
       <c r="C281" s="114" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D281" s="114"/>
       <c r="E281" s="114"/>
@@ -19237,7 +19238,7 @@
     </row>
     <row r="288" spans="1:14" ht="14.45" customHeight="1">
       <c r="A288" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B288" s="2"/>
       <c r="C288" s="2"/>
@@ -19295,7 +19296,7 @@
       </c>
       <c r="B291" s="2"/>
       <c r="C291" s="100" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D291" s="100"/>
       <c r="E291" s="100"/>
@@ -19376,7 +19377,7 @@
         <v>5</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
@@ -19396,7 +19397,7 @@
         <v>5</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>

</xml_diff>

<commit_message>
pm_pcsgen: Make it possible to specify a custom clone ID
</commit_message>
<xml_diff>
--- a/pm_pcsgen/pm_pcsgen_sample.xlsx
+++ b/pm_pcsgen/pm_pcsgen_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ka_inoue\Desktop\telwork\UPD\4802_4786\4786\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ka_inoue\Desktop\telwork\UPD\4802_4786\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1534" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="254">
   <si>
     <t>NODE</t>
   </si>
@@ -1041,71 +1041,6 @@
         <family val="1"/>
       </rPr>
       <t>ID</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Clone</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>の</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>には「</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>&lt;Clone</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>対象リソースの</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>ID&gt;-clone</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>」を指定すること</t>
     </r>
   </si>
   <si>
@@ -2433,71 +2368,6 @@
         <charset val="128"/>
       </rPr>
       <t>」を記述する。</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Promotable</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>の</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>には「</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>&lt;Promotable</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>対象リソースの</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>ID&gt;-clone</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="メイリオ"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>」を指定すること</t>
     </r>
   </si>
   <si>
@@ -6465,7 +6335,7 @@
               <a:latin typeface="メイリオ"/>
               <a:ea typeface="メイリオ"/>
             </a:rPr>
-            <a:t>Copyright (C) 2020 NIPPON TELEGRAPH AND TELEPHONE CORPORATION</a:t>
+            <a:t>Copyright (C) 2020-2021 NIPPON TELEGRAPH AND TELEPHONE CORPORATION</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="800" b="0" strike="noStrike" spc="-1">
             <a:latin typeface="Times New Roman"/>
@@ -6647,7 +6517,7 @@
               <a:latin typeface="メイリオ"/>
               <a:ea typeface="メイリオ"/>
             </a:rPr>
-            <a:t>Copyright (C) 2020 NIPPON TELEGRAPH AND TELEPHONE CORPORATION</a:t>
+            <a:t>Copyright (C) 2020-2021 NIPPON TELEGRAPH AND TELEPHONE CORPORATION</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="800" b="0" strike="noStrike" spc="-1">
             <a:latin typeface="Times New Roman"/>
@@ -7727,9 +7597,7 @@
       <c r="I41" s="207"/>
       <c r="J41" s="207"/>
       <c r="K41" s="207"/>
-      <c r="L41" s="208" t="s">
-        <v>211</v>
-      </c>
+      <c r="L41" s="208"/>
       <c r="M41" s="208"/>
       <c r="N41" s="208"/>
     </row>
@@ -7807,7 +7675,7 @@
     </row>
     <row r="46" spans="1:14" ht="14.45" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -7942,7 +7810,7 @@
     </row>
     <row r="53" spans="1:14" ht="14.45" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -8004,16 +7872,16 @@
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="188" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D56" s="188"/>
       <c r="E56" s="189" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F56" s="189"/>
       <c r="G56" s="189"/>
       <c r="H56" s="190" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I56" s="190"/>
       <c r="J56" s="190"/>
@@ -8086,7 +7954,7 @@
     </row>
     <row r="61" spans="1:14" ht="14.45" customHeight="1">
       <c r="A61" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -8361,26 +8229,26 @@
       </c>
       <c r="B73" s="26"/>
       <c r="C73" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D73" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D73" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E73" s="123"/>
       <c r="F73" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G73" s="123"/>
       <c r="H73" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I73" s="108"/>
       <c r="J73" s="108" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K73" s="108"/>
       <c r="L73" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M73" s="179" t="s">
         <v>201</v>
@@ -8726,26 +8594,26 @@
       </c>
       <c r="B89" s="26"/>
       <c r="C89" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D89" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D89" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E89" s="123"/>
       <c r="F89" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G89" s="123"/>
       <c r="H89" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I89" s="108"/>
       <c r="J89" s="108" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K89" s="108"/>
       <c r="L89" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M89" s="179" t="s">
         <v>201</v>
@@ -9091,26 +8959,26 @@
       </c>
       <c r="B105" s="26"/>
       <c r="C105" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D105" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D105" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E105" s="123"/>
       <c r="F105" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G105" s="123"/>
       <c r="H105" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I105" s="108"/>
       <c r="J105" s="108" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K105" s="108"/>
       <c r="L105" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M105" s="179" t="s">
         <v>201</v>
@@ -9437,26 +9305,26 @@
       </c>
       <c r="B120" s="26"/>
       <c r="C120" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D120" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D120" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E120" s="123"/>
       <c r="F120" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G120" s="123"/>
       <c r="H120" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I120" s="108"/>
       <c r="J120" s="108" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K120" s="108"/>
       <c r="L120" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M120" s="179" t="s">
         <v>201</v>
@@ -9840,26 +9708,26 @@
       </c>
       <c r="B138" s="26"/>
       <c r="C138" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D138" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D138" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E138" s="123"/>
       <c r="F138" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G138" s="123"/>
       <c r="H138" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I138" s="108"/>
       <c r="J138" s="108" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K138" s="108"/>
       <c r="L138" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M138" s="179" t="s">
         <v>201</v>
@@ -10224,26 +10092,26 @@
       </c>
       <c r="B155" s="26"/>
       <c r="C155" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D155" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D155" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E155" s="123"/>
       <c r="F155" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G155" s="123"/>
       <c r="H155" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I155" s="108"/>
       <c r="J155" s="108" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K155" s="108"/>
       <c r="L155" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M155" s="179" t="s">
         <v>201</v>
@@ -10332,7 +10200,7 @@
     </row>
     <row r="160" spans="1:14" ht="14.45" customHeight="1">
       <c r="A160" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -10394,7 +10262,7 @@
       </c>
       <c r="B163" s="26"/>
       <c r="C163" s="127" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D163" s="127"/>
       <c r="E163" s="182" t="s">
@@ -10517,7 +10385,7 @@
       <c r="I168" s="134"/>
       <c r="J168" s="134"/>
       <c r="K168" s="119" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L168" s="119"/>
       <c r="M168" s="119"/>
@@ -10612,18 +10480,18 @@
       </c>
       <c r="B173" s="26"/>
       <c r="C173" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D173" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D173" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E173" s="123"/>
       <c r="F173" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G173" s="123"/>
       <c r="H173" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I173" s="108"/>
       <c r="J173" s="108"/>
@@ -10760,7 +10628,7 @@
       </c>
       <c r="B180" s="26"/>
       <c r="C180" s="127" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D180" s="127"/>
       <c r="E180" s="182" t="s">
@@ -10883,7 +10751,7 @@
       <c r="I185" s="134"/>
       <c r="J185" s="134"/>
       <c r="K185" s="119" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L185" s="119"/>
       <c r="M185" s="119"/>
@@ -10978,18 +10846,18 @@
       </c>
       <c r="B190" s="26"/>
       <c r="C190" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D190" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D190" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E190" s="123"/>
       <c r="F190" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G190" s="123"/>
       <c r="H190" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I190" s="108"/>
       <c r="J190" s="108"/>
@@ -11082,7 +10950,7 @@
     </row>
     <row r="195" spans="1:14" ht="14.45" customHeight="1">
       <c r="A195" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
@@ -11153,15 +11021,15 @@
       </c>
       <c r="F198" s="163"/>
       <c r="G198" s="164" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H198" s="164"/>
       <c r="I198" s="165" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J198" s="165"/>
       <c r="K198" s="166" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L198" s="166"/>
       <c r="M198" s="166"/>
@@ -11268,7 +11136,7 @@
     </row>
     <row r="204" spans="1:14" ht="14.45" customHeight="1">
       <c r="A204" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
@@ -11342,24 +11210,24 @@
       </c>
       <c r="D207" s="127"/>
       <c r="E207" s="49" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F207" s="50" t="s">
         <v>123</v>
       </c>
       <c r="G207" s="153" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H207" s="153"/>
       <c r="I207" s="51" t="s">
+        <v>232</v>
+      </c>
+      <c r="J207" s="154" t="s">
         <v>233</v>
-      </c>
-      <c r="J207" s="154" t="s">
-        <v>234</v>
       </c>
       <c r="K207" s="154"/>
       <c r="L207" s="52" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M207" s="155" t="s">
         <v>201</v>
@@ -11444,7 +11312,7 @@
     </row>
     <row r="212" spans="1:14" ht="14.45" customHeight="1">
       <c r="A212" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
@@ -11510,23 +11378,23 @@
       </c>
       <c r="B215" s="2"/>
       <c r="C215" s="127" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D215" s="127"/>
       <c r="E215" s="128" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F215" s="128"/>
       <c r="G215" s="136" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H215" s="136"/>
       <c r="I215" s="128" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J215" s="128"/>
       <c r="K215" s="128" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L215" s="128"/>
       <c r="M215" s="101" t="s">
@@ -11602,7 +11470,7 @@
     </row>
     <row r="220" spans="1:14" ht="14.45" customHeight="1">
       <c r="A220" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
@@ -11670,11 +11538,11 @@
       </c>
       <c r="B223" s="2"/>
       <c r="C223" s="127" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D223" s="127"/>
       <c r="E223" s="128" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F223" s="128"/>
       <c r="G223" s="128" t="s">
@@ -11682,15 +11550,15 @@
       </c>
       <c r="H223" s="128"/>
       <c r="I223" s="128" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J223" s="128"/>
       <c r="K223" s="128" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L223" s="128"/>
       <c r="M223" s="49" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="N223" s="66" t="s">
         <v>201</v>
@@ -11764,7 +11632,7 @@
     </row>
     <row r="228" spans="1:14" ht="14.45" customHeight="1">
       <c r="A228" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
@@ -11824,7 +11692,7 @@
       </c>
       <c r="B231" s="26"/>
       <c r="C231" s="121" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D231" s="121"/>
       <c r="E231" s="121"/>
@@ -11961,7 +11829,7 @@
       </c>
       <c r="B238" s="26"/>
       <c r="C238" s="114" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D238" s="114"/>
       <c r="E238" s="114"/>
@@ -12098,7 +11966,7 @@
       </c>
       <c r="B245" s="26"/>
       <c r="C245" s="114" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D245" s="114"/>
       <c r="E245" s="114"/>
@@ -12226,7 +12094,7 @@
     </row>
     <row r="252" spans="1:14" ht="14.45" customHeight="1">
       <c r="A252" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
@@ -12284,7 +12152,7 @@
       </c>
       <c r="B255" s="2"/>
       <c r="C255" s="100" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D255" s="100"/>
       <c r="E255" s="100"/>
@@ -12365,7 +12233,7 @@
         <v>5</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
@@ -12385,7 +12253,7 @@
         <v>5</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
@@ -13914,9 +13782,7 @@
       <c r="I39" s="124"/>
       <c r="J39" s="124"/>
       <c r="K39" s="124"/>
-      <c r="L39" s="208" t="s">
-        <v>253</v>
-      </c>
+      <c r="L39" s="208"/>
       <c r="M39" s="208"/>
       <c r="N39" s="208"/>
     </row>
@@ -13954,9 +13820,7 @@
       <c r="I41" s="207"/>
       <c r="J41" s="207"/>
       <c r="K41" s="207"/>
-      <c r="L41" s="208" t="s">
-        <v>211</v>
-      </c>
+      <c r="L41" s="208"/>
       <c r="M41" s="208"/>
       <c r="N41" s="208"/>
     </row>
@@ -14110,7 +13974,7 @@
     </row>
     <row r="50" spans="1:14" ht="14.45" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -14325,7 +14189,7 @@
     </row>
     <row r="61" spans="1:14" ht="14.45" customHeight="1">
       <c r="A61" s="84" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -14387,16 +14251,16 @@
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="188" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D64" s="188"/>
       <c r="E64" s="189" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F64" s="189"/>
       <c r="G64" s="189"/>
       <c r="H64" s="190" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I64" s="190"/>
       <c r="J64" s="190"/>
@@ -14504,7 +14368,7 @@
     </row>
     <row r="70" spans="1:14" ht="14.45" customHeight="1">
       <c r="A70" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -14760,26 +14624,26 @@
       </c>
       <c r="B81" s="26"/>
       <c r="C81" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D81" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D81" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E81" s="123"/>
       <c r="F81" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G81" s="123"/>
       <c r="H81" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I81" s="108"/>
       <c r="J81" s="108" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K81" s="108"/>
       <c r="L81" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M81" s="238" t="s">
         <v>201</v>
@@ -15127,26 +14991,26 @@
       </c>
       <c r="B97" s="26"/>
       <c r="C97" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D97" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D97" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E97" s="123"/>
       <c r="F97" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G97" s="123"/>
       <c r="H97" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I97" s="108"/>
       <c r="J97" s="108" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K97" s="108"/>
       <c r="L97" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M97" s="238" t="s">
         <v>201</v>
@@ -15494,26 +15358,26 @@
       </c>
       <c r="B113" s="26"/>
       <c r="C113" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D113" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D113" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E113" s="123"/>
       <c r="F113" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G113" s="123"/>
       <c r="H113" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I113" s="108"/>
       <c r="J113" s="108" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K113" s="108"/>
       <c r="L113" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M113" s="238" t="s">
         <v>201</v>
@@ -16049,26 +15913,26 @@
       </c>
       <c r="B139" s="26"/>
       <c r="C139" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D139" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D139" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E139" s="123"/>
       <c r="F139" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G139" s="123"/>
       <c r="H139" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I139" s="108"/>
       <c r="J139" s="108" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K139" s="108"/>
       <c r="L139" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M139" s="238" t="s">
         <v>201</v>
@@ -16519,26 +16383,26 @@
       </c>
       <c r="B160" s="26"/>
       <c r="C160" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D160" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D160" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E160" s="123"/>
       <c r="F160" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G160" s="123"/>
       <c r="H160" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I160" s="108"/>
       <c r="J160" s="108" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K160" s="108"/>
       <c r="L160" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M160" s="238" t="s">
         <v>201</v>
@@ -16627,7 +16491,7 @@
     </row>
     <row r="165" spans="1:14" ht="14.25" customHeight="1">
       <c r="A165" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -16848,18 +16712,18 @@
       </c>
       <c r="B175" s="26"/>
       <c r="C175" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D175" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D175" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E175" s="123"/>
       <c r="F175" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G175" s="123"/>
       <c r="H175" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I175" s="108"/>
       <c r="J175" s="108"/>
@@ -17155,18 +17019,18 @@
       </c>
       <c r="B189" s="26"/>
       <c r="C189" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D189" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D189" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E189" s="123"/>
       <c r="F189" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G189" s="123"/>
       <c r="H189" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I189" s="108"/>
       <c r="J189" s="108"/>
@@ -17426,7 +17290,7 @@
       <c r="I201" s="134"/>
       <c r="J201" s="134"/>
       <c r="K201" s="119" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L201" s="119"/>
       <c r="M201" s="119"/>
@@ -17521,18 +17385,18 @@
       </c>
       <c r="B206" s="26"/>
       <c r="C206" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D206" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D206" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E206" s="123"/>
       <c r="F206" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G206" s="123"/>
       <c r="H206" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I206" s="108"/>
       <c r="J206" s="108"/>
@@ -17792,7 +17656,7 @@
       <c r="I218" s="134"/>
       <c r="J218" s="134"/>
       <c r="K218" s="119" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L218" s="119"/>
       <c r="M218" s="119"/>
@@ -17887,18 +17751,18 @@
       </c>
       <c r="B223" s="26"/>
       <c r="C223" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D223" s="123" t="s">
         <v>218</v>
-      </c>
-      <c r="D223" s="123" t="s">
-        <v>219</v>
       </c>
       <c r="E223" s="123"/>
       <c r="F223" s="123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G223" s="123"/>
       <c r="H223" s="108" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I223" s="108"/>
       <c r="J223" s="108"/>
@@ -17991,7 +17855,7 @@
     </row>
     <row r="228" spans="1:14" ht="14.45" customHeight="1">
       <c r="A228" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
@@ -18062,15 +17926,15 @@
       </c>
       <c r="F231" s="163"/>
       <c r="G231" s="164" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H231" s="164"/>
       <c r="I231" s="165" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J231" s="165"/>
       <c r="K231" s="166" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L231" s="166"/>
       <c r="M231" s="166"/>
@@ -18150,7 +18014,7 @@
     </row>
     <row r="236" spans="1:14" ht="14.45" customHeight="1">
       <c r="A236" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
@@ -18224,24 +18088,24 @@
       </c>
       <c r="D239" s="162"/>
       <c r="E239" s="49" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F239" s="50" t="s">
         <v>123</v>
       </c>
       <c r="G239" s="153" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H239" s="153"/>
       <c r="I239" s="51" t="s">
+        <v>232</v>
+      </c>
+      <c r="J239" s="154" t="s">
         <v>233</v>
-      </c>
-      <c r="J239" s="154" t="s">
-        <v>234</v>
       </c>
       <c r="K239" s="154"/>
       <c r="L239" s="52" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="M239" s="155" t="s">
         <v>201</v>
@@ -18426,7 +18290,7 @@
     </row>
     <row r="248" spans="1:14" ht="14.45" customHeight="1">
       <c r="A248" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
@@ -18492,23 +18356,23 @@
       </c>
       <c r="B251" s="2"/>
       <c r="C251" s="127" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D251" s="127"/>
       <c r="E251" s="128" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F251" s="128"/>
       <c r="G251" s="136" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H251" s="136"/>
       <c r="I251" s="128" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J251" s="128"/>
       <c r="K251" s="128" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L251" s="128"/>
       <c r="M251" s="101" t="s">
@@ -18592,7 +18456,7 @@
     </row>
     <row r="256" spans="1:14" ht="14.45" customHeight="1">
       <c r="A256" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
@@ -18660,11 +18524,11 @@
       </c>
       <c r="B259" s="2"/>
       <c r="C259" s="127" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D259" s="127"/>
       <c r="E259" s="128" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F259" s="128"/>
       <c r="G259" s="128" t="s">
@@ -18672,15 +18536,15 @@
       </c>
       <c r="H259" s="128"/>
       <c r="I259" s="128" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J259" s="128"/>
       <c r="K259" s="128" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L259" s="128"/>
       <c r="M259" s="49" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="N259" s="66" t="s">
         <v>201</v>
@@ -18776,7 +18640,7 @@
     </row>
     <row r="264" spans="1:14" ht="14.45" customHeight="1">
       <c r="A264" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
@@ -18836,7 +18700,7 @@
       </c>
       <c r="B267" s="26"/>
       <c r="C267" s="121" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D267" s="121"/>
       <c r="E267" s="121"/>
@@ -18973,7 +18837,7 @@
       </c>
       <c r="B274" s="26"/>
       <c r="C274" s="114" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D274" s="114"/>
       <c r="E274" s="114"/>
@@ -19110,7 +18974,7 @@
       </c>
       <c r="B281" s="26"/>
       <c r="C281" s="114" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D281" s="114"/>
       <c r="E281" s="114"/>
@@ -19238,7 +19102,7 @@
     </row>
     <row r="288" spans="1:14" ht="14.45" customHeight="1">
       <c r="A288" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B288" s="2"/>
       <c r="C288" s="2"/>
@@ -19296,7 +19160,7 @@
       </c>
       <c r="B291" s="2"/>
       <c r="C291" s="100" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D291" s="100"/>
       <c r="E291" s="100"/>
@@ -19377,7 +19241,7 @@
         <v>5</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
@@ -19397,7 +19261,7 @@
         <v>5</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>

</xml_diff>